<commit_message>
updated sheet name from composite to evaluation
</commit_message>
<xml_diff>
--- a/Preliminary-Evaluation/nl4dv-llm-evaluation.xlsx
+++ b/Preliminary-Evaluation/nl4dv-llm-evaluation.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subham.sah\Desktop\NLVIZV3\camera ready\supplemental material\suplementary materials\Preliminary-Evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subham.sah\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34699A7-112D-4746-8B30-73603A9B8BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671F2ACF-F9FA-4B47-8C6F-77128F2783D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Composite_NL4DV-LLM" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="NL4DV-LLM Evaluation" sheetId="1" r:id="rId1"/>
+    <sheet name="NL4DV Evaluation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2704,7 +2704,7 @@
   </sheetPr>
   <dimension ref="A1:R991"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -27513,7 +27513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0D09A8-0072-42C7-9FB1-3248CDAEA0F9}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>

</xml_diff>